<commit_message>
P11 Saunalahti -> Espoonlahden koulu
</commit_message>
<xml_diff>
--- a/Poikkeusvuorot vko13.xlsx
+++ b/Poikkeusvuorot vko13.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="118">
   <si>
     <t>VAKIOVUOROT 2021-23</t>
   </si>
@@ -189,7 +189,7 @@
     <t>17-18.45</t>
   </si>
   <si>
-    <t>17-19.30</t>
+    <t>17-19</t>
   </si>
   <si>
     <t>Hede</t>
@@ -210,7 +210,16 @@
     <t>18.45-20</t>
   </si>
   <si>
+    <t>19-20.15</t>
+  </si>
+  <si>
+    <t>P11</t>
+  </si>
+  <si>
     <t>19.30-21.30</t>
+  </si>
+  <si>
+    <t>20.15-21.30</t>
   </si>
   <si>
     <t>18.00-20.00</t>
@@ -229,9 +238,6 @@
   </si>
   <si>
     <t>17.00-19.00</t>
-  </si>
-  <si>
-    <t>P11</t>
   </si>
   <si>
     <t>10.00-16.00</t>
@@ -255,16 +261,10 @@
     <t>Karhusuo</t>
   </si>
   <si>
-    <t>19-20.15</t>
-  </si>
-  <si>
     <t>Tomppa</t>
   </si>
   <si>
     <t>9.00-12.00</t>
-  </si>
-  <si>
-    <t>20.15-21.30</t>
   </si>
   <si>
     <t>Farmi</t>
@@ -277,9 +277,6 @@
   </si>
   <si>
     <t>Koriskoulu</t>
-  </si>
-  <si>
-    <t>17-19</t>
   </si>
   <si>
     <t>09.00-10.00</t>
@@ -340,9 +337,6 @@
   </si>
   <si>
     <t>NKL/T07</t>
-  </si>
-  <si>
-    <t>19-21.30</t>
   </si>
   <si>
     <t>Storängens Skola</t>
@@ -1445,7 +1439,7 @@
         <v>64</v>
       </c>
       <c r="K14" s="32" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="L14" s="36" t="s">
         <v>48</v>
@@ -1482,11 +1476,15 @@
       </c>
       <c r="G15" s="18"/>
       <c r="H15" s="31" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I15" s="14"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
+      <c r="J15" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="K15" s="32" t="s">
+        <v>51</v>
+      </c>
       <c r="L15" s="36" t="s">
         <v>53</v>
       </c>
@@ -1560,16 +1558,16 @@
       <c r="J17" s="23"/>
       <c r="K17" s="23"/>
       <c r="L17" s="36" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="M17" s="36" t="s">
         <v>58</v>
       </c>
       <c r="N17" s="37" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="O17" s="37" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="P17" s="9"/>
       <c r="Q17" s="9"/>
@@ -1641,19 +1639,19 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E20" s="38" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
@@ -1664,10 +1662,10 @@
       <c r="L20" s="17"/>
       <c r="M20" s="17"/>
       <c r="N20" s="18" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="O20" s="25" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="P20" s="9"/>
       <c r="Q20" s="9"/>
@@ -1687,7 +1685,7 @@
         <v>46</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
@@ -1799,7 +1797,7 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B25" s="19" t="s">
         <v>38</v>
@@ -1816,11 +1814,11 @@
       <c r="J25" s="23"/>
       <c r="K25" s="23"/>
       <c r="L25" s="16" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="M25" s="16"/>
       <c r="N25" s="18" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="O25" s="18"/>
       <c r="P25" s="9"/>
@@ -1852,11 +1850,11 @@
       <c r="J26" s="23"/>
       <c r="K26" s="15"/>
       <c r="L26" s="16" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M26" s="16"/>
       <c r="N26" s="18" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="O26" s="18"/>
       <c r="P26" s="9"/>
@@ -1888,11 +1886,11 @@
       <c r="J27" s="15"/>
       <c r="K27" s="15"/>
       <c r="L27" s="16" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="M27" s="16"/>
       <c r="N27" s="18" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="O27" s="18"/>
       <c r="P27" s="9"/>
@@ -1965,7 +1963,7 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -1975,21 +1973,21 @@
         <v>36</v>
       </c>
       <c r="G30" s="18" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="H30" s="22"/>
       <c r="I30" s="22"/>
       <c r="J30" s="23" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="K30" s="39" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L30" s="16" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M30" s="34" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N30" s="13"/>
       <c r="O30" s="13"/>
@@ -2015,15 +2013,15 @@
         <v>43</v>
       </c>
       <c r="G31" s="18" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="H31" s="22"/>
       <c r="I31" s="22"/>
       <c r="J31" s="23" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="K31" s="39" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L31" s="17"/>
       <c r="M31" s="17"/>
@@ -2148,7 +2146,7 @@
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
       <c r="H35" s="22" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="I35" s="31" t="s">
         <v>58</v>
@@ -2157,19 +2155,19 @@
         <v>39</v>
       </c>
       <c r="K35" s="39" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L35" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="M35" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="M35" s="34" t="s">
-        <v>89</v>
-      </c>
       <c r="N35" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O35" s="30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P35" s="9"/>
       <c r="Q35" s="9"/>
@@ -2192,7 +2190,7 @@
         <v>58</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E36" s="38" t="s">
         <v>86</v>
@@ -2200,7 +2198,7 @@
       <c r="F36" s="18"/>
       <c r="G36" s="18"/>
       <c r="H36" s="22" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="I36" s="29" t="s">
         <v>58</v>
@@ -2215,13 +2213,13 @@
         <v>42</v>
       </c>
       <c r="M36" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="N36" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="N36" s="42" t="s">
-        <v>93</v>
-      </c>
       <c r="O36" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P36" s="9"/>
       <c r="Q36" s="9"/>
@@ -2248,19 +2246,19 @@
       <c r="F37" s="18"/>
       <c r="G37" s="13"/>
       <c r="H37" s="22" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="I37" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J37" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K37" s="39" t="s">
         <v>59</v>
       </c>
       <c r="L37" s="34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M37" s="17"/>
       <c r="N37" s="13"/>
@@ -2335,7 +2333,7 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -2343,23 +2341,23 @@
         <v>38</v>
       </c>
       <c r="E40" s="38" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F40" s="13"/>
       <c r="G40" s="13"/>
       <c r="H40" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I40" s="22" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="J40" s="23"/>
       <c r="K40" s="23"/>
       <c r="L40" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M40" s="16" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="N40" s="18"/>
       <c r="O40" s="18"/>
@@ -2383,7 +2381,7 @@
         <v>62</v>
       </c>
       <c r="E41" s="38" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
@@ -2391,7 +2389,7 @@
         <v>46</v>
       </c>
       <c r="I41" s="22" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="J41" s="23"/>
       <c r="K41" s="23"/>
@@ -2469,7 +2467,7 @@
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -2485,13 +2483,13 @@
         <v>42</v>
       </c>
       <c r="M44" s="16" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="N44" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O44" s="18" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="P44" s="9"/>
       <c r="Q44" s="9"/>
@@ -2518,10 +2516,10 @@
       <c r="J45" s="15"/>
       <c r="K45" s="15"/>
       <c r="L45" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M45" s="16" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="N45" s="18"/>
       <c r="O45" s="18"/>
@@ -2539,7 +2537,7 @@
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
@@ -2548,7 +2546,7 @@
       <c r="F46" s="13"/>
       <c r="G46" s="13"/>
       <c r="H46" s="22" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="I46" s="29" t="s">
         <v>59</v>
@@ -2580,10 +2578,10 @@
       <c r="F47" s="13"/>
       <c r="G47" s="13"/>
       <c r="H47" s="22" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="I47" s="31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J47" s="23"/>
       <c r="K47" s="15"/>
@@ -2633,10 +2631,10 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B49" s="41" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C49" s="41" t="s">
         <v>59</v>
@@ -2723,7 +2721,7 @@
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B52" s="11"/>
       <c r="C52" s="11"/>
@@ -2735,14 +2733,10 @@
         <v>49</v>
       </c>
       <c r="I52" s="29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
-      <c r="J52" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="K52" s="32" t="s">
-        <v>71</v>
-      </c>
+      <c r="J52" s="32"/>
+      <c r="K52" s="32"/>
       <c r="L52" s="17"/>
       <c r="M52" s="17"/>
       <c r="N52" s="13"/>
@@ -2817,13 +2811,13 @@
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="40" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B55" s="19" t="s">
         <v>39</v>
       </c>
       <c r="C55" s="41" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D55" s="12"/>
       <c r="E55" s="12"/>
@@ -2837,13 +2831,13 @@
         <v>42</v>
       </c>
       <c r="M55" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N55" s="18" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="O55" s="25" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="P55" s="9"/>
       <c r="Q55" s="9"/>
@@ -2863,7 +2857,7 @@
         <v>61</v>
       </c>
       <c r="C56" s="41" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D56" s="12"/>
       <c r="E56" s="12"/>
@@ -2919,26 +2913,26 @@
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B58" s="26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D58" s="12"/>
       <c r="E58" s="12"/>
       <c r="F58" s="30" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="G58" s="30" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H58" s="14"/>
       <c r="I58" s="14"/>
       <c r="J58" s="15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K58" s="39" t="s">
         <v>60</v>
@@ -2962,18 +2956,18 @@
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="10"/>
       <c r="B59" s="26" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="C59" s="26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D59" s="12"/>
       <c r="E59" s="38"/>
       <c r="F59" s="30" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="G59" s="30" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H59" s="14"/>
       <c r="I59" s="14"/>
@@ -3025,19 +3019,19 @@
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C61" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="B61" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="C61" s="41" t="s">
-        <v>117</v>
-      </c>
       <c r="D61" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F61" s="13"/>
       <c r="G61" s="13"/>
@@ -3069,7 +3063,7 @@
         <v>30</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F62" s="13"/>
       <c r="G62" s="13"/>

</xml_diff>